<commit_message>
Added Company Accounts for year end March 2024
</commit_message>
<xml_diff>
--- a/GB Accounts 2023-24/GB Accounts Company 2024-03-31 (Mar24) Excel 2007/Companysecretary.xlsx
+++ b/GB Accounts 2023-24/GB Accounts Company 2024-03-31 (Mar24) Excel 2007/Companysecretary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Downloads\GB Accounts Company 2023-03-31 (Mar23) Excel 2007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony/projects/diy-accounting/GB Accounts 2023-24/GB Accounts Company 2024-03-31 (Mar24) Excel 2007/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D786151D-EDB3-4395-8445-CE981CDEA725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580F5602-F421-D74A-87F0-575876BF86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boardmeeting" sheetId="5" r:id="rId1"/>
@@ -173,10 +173,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -187,6 +189,7 @@
       <sz val="9"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -649,18 +652,18 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="24" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="24"/>
-    <col min="4" max="4" width="12.5703125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="28"/>
-    <col min="6" max="6" width="14.42578125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" style="24" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="1.6640625" style="24" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" style="24"/>
+    <col min="4" max="4" width="12.5" style="24" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="28"/>
+    <col min="6" max="6" width="14.5" style="24" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" style="24" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -669,7 +672,7 @@
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="22"/>
       <c r="B2" s="29" t="s">
         <v>36</v>
@@ -680,7 +683,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -689,7 +692,7 @@
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="22"/>
       <c r="B4" s="22" t="s">
         <v>35</v>
@@ -700,7 +703,7 @@
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -709,7 +712,7 @@
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="22"/>
       <c r="B6" s="22" t="s">
         <v>34</v>
@@ -722,7 +725,7 @@
       </c>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -731,7 +734,7 @@
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="22"/>
       <c r="B8" s="27" t="str">
         <f>IF(E8&gt;0,"UPDATE REGISTERMEMBERS"," ")</f>
@@ -745,7 +748,7 @@
       </c>
       <c r="G8" s="22"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -754,7 +757,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="22"/>
       <c r="B10" s="22" t="s">
         <v>33</v>
@@ -765,7 +768,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
     </row>
-    <row r="11" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -799,17 +802,17 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="19.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="2" width="19.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -829,7 +832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
@@ -837,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
@@ -867,22 +870,22 @@
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="6" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="10" max="10" width="10.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -903,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="21" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="21" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -935,7 +938,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
@@ -952,7 +955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="D4" s="11" t="s">
         <v>17</v>
       </c>
@@ -991,17 +994,17 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="23" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="6"/>
+    <col min="5" max="5" width="25.5" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="D2" s="6" t="s">
         <v>22</v>
       </c>
@@ -1048,18 +1051,18 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="12.6640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="18" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>24</v>
       </c>

</xml_diff>